<commit_message>
A lot of things added current task(start screen/menu)
</commit_message>
<xml_diff>
--- a/MapGen.xlsx
+++ b/MapGen.xlsx
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="2">
   <si>
     <t>w</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -84,7 +87,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -93,9 +96,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -109,7 +115,50 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0070C0"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -123,7 +172,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0070C0"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -135,9 +184,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -461,7 +513,7 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +553,7 @@
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="2">
         <v>0</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -539,62 +591,62 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>0</v>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>2</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>2</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>3</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>0</v>
@@ -604,61 +656,61 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>2</v>
+      <c r="L3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="N3" s="2">
         <v>0</v>
       </c>
-      <c r="O3" s="2">
-        <v>2</v>
+      <c r="O3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="P3" s="2">
         <v>0</v>
       </c>
       <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
-        <v>2</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
         <v>0</v>
       </c>
       <c r="U3" s="2" t="s">
@@ -669,62 +721,62 @@
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
+      <c r="B4" s="2">
+        <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
         <v>0</v>
       </c>
       <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2">
         <v>0</v>
       </c>
       <c r="P4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>0</v>
+      <c r="R4" s="2">
+        <v>2</v>
       </c>
       <c r="S4" s="2">
-        <v>2</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>2</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>0</v>
@@ -737,58 +789,58 @@
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>2</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>2</v>
-      </c>
-      <c r="O5" s="2">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="P5" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="R5" s="2">
-        <v>2</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
         <v>0</v>
       </c>
       <c r="U5" s="2" t="s">
@@ -799,129 +851,129 @@
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
+      <c r="B6" s="2">
+        <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
         <v>0</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2">
         <v>0</v>
       </c>
       <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2">
         <v>0</v>
       </c>
       <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2">
-        <v>3</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>2</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>2</v>
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>2</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="M7" s="2">
         <v>2</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P7" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="2">
+      <c r="P7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="R7" s="2">
-        <v>2</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
         <v>0</v>
       </c>
     </row>
@@ -929,62 +981,62 @@
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="2">
         <v>0</v>
       </c>
       <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>4</v>
       </c>
       <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>2</v>
+      </c>
+      <c r="O8" s="2">
         <v>0</v>
       </c>
       <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>4</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="2" t="s">
-        <v>0</v>
+      <c r="T8" s="2">
+        <v>2</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>0</v>
@@ -997,58 +1049,58 @@
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2</v>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="I9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J9" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9" s="2">
-        <v>2</v>
-      </c>
-      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N9" s="2">
-        <v>2</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="Q9" s="2">
-        <v>0</v>
-      </c>
-      <c r="R9" s="2">
-        <v>2</v>
-      </c>
-      <c r="S9" s="2">
-        <v>0</v>
-      </c>
-      <c r="T9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
         <v>0</v>
       </c>
       <c r="U9" s="2" t="s">
@@ -1059,62 +1111,62 @@
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>0</v>
+      <c r="B10" s="2">
+        <v>2</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
         <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="2">
         <v>0</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K10" s="2">
-        <v>2</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>0</v>
+      <c r="K10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>2</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>2</v>
       </c>
       <c r="S10" s="2">
-        <v>2</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>3</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>0</v>
@@ -1124,14 +1176,14 @@
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>0</v>
@@ -1146,36 +1198,36 @@
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="O11" s="2">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" s="2">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2">
+        <v>2</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>2</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="T11" s="2" t="s">
@@ -1186,20 +1238,20 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>0</v>
+      <c r="A12" s="2">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
@@ -1207,14 +1259,14 @@
       <c r="G12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="2">
-        <v>2</v>
+      <c r="H12" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>0</v>
+      <c r="J12" s="2">
+        <v>2</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>0</v>
@@ -1225,28 +1277,28 @@
       <c r="M12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N12" s="2">
-        <v>0</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="2" t="s">
+      <c r="N12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
         <v>0</v>
       </c>
       <c r="R12" s="2">
         <v>2</v>
       </c>
-      <c r="S12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U12" s="2" t="s">
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
+        <v>2</v>
+      </c>
+      <c r="U12" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1254,29 +1306,29 @@
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>0</v>
+      <c r="G13" s="2">
+        <v>2</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
       </c>
-      <c r="I13" s="2">
-        <v>3</v>
+      <c r="I13" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="J13" s="2">
         <v>0</v>
@@ -1285,30 +1337,30 @@
         <v>0</v>
       </c>
       <c r="L13" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13" s="2">
-        <v>3</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>2</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="R13" s="2">
         <v>0</v>
       </c>
-      <c r="S13" s="2">
-        <v>0</v>
-      </c>
-      <c r="T13" s="2" t="s">
+      <c r="S13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
         <v>0</v>
       </c>
       <c r="U13" s="2" t="s">
@@ -1319,38 +1371,38 @@
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>0</v>
+      <c r="B14" s="2">
+        <v>2</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>0</v>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2" t="s">
+      <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
         <v>0</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>0</v>
@@ -1358,23 +1410,23 @@
       <c r="N14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="2">
         <v>0</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S14" s="2">
-        <v>0</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>2</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>2</v>
       </c>
       <c r="U14" s="2" t="s">
         <v>0</v>
@@ -1384,41 +1436,41 @@
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3</v>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>2</v>
+      <c r="E15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H15" s="2">
         <v>0</v>
       </c>
-      <c r="I15" s="2">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2</v>
+      <c r="I15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L15" s="2">
         <v>0</v>
       </c>
-      <c r="M15" s="2">
-        <v>2</v>
+      <c r="M15" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="N15" s="2">
         <v>0</v>
@@ -1429,16 +1481,16 @@
       <c r="P15" s="2">
         <v>0</v>
       </c>
-      <c r="Q15" s="2">
-        <v>2</v>
-      </c>
-      <c r="R15" s="2">
-        <v>0</v>
-      </c>
-      <c r="S15" s="2">
-        <v>3</v>
-      </c>
-      <c r="T15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
         <v>0</v>
       </c>
       <c r="U15" s="2" t="s">
@@ -1449,62 +1501,62 @@
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>0</v>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2">
+        <v>2</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2">
+        <v>3</v>
       </c>
       <c r="U16" s="2" t="s">
         <v>0</v>
@@ -1541,7 +1593,7 @@
       <c r="J17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="2">
         <v>0</v>
       </c>
       <c r="L17" s="2" t="s">
@@ -1578,20 +1630,26 @@
     <row r="18" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:U17">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="0">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="0">
       <formula>NOT(ISERROR(SEARCH("0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="s">
+      <formula>NOT(ISERROR(SEARCH("s",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="4">
+      <formula>NOT(ISERROR(SEARCH("4",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>